<commit_message>
Added two new fields.
</commit_message>
<xml_diff>
--- a/static/fields/devicecovid19serology_reference.xlsx
+++ b/static/fields/devicecovid19serology_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E4D85-94BE-5941-B5D1-D2290926F1EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BB762D-08DC-3345-8607-BC91DF276A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1080" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Field Name</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>The unique identifier for each evaluation.</t>
+  </si>
+  <si>
+    <t>igm_iga_agree</t>
+  </si>
+  <si>
+    <t>Agreement between igm_iga_result and antibody_truth.</t>
+  </si>
+  <si>
+    <t>igm_iga_result</t>
+  </si>
+  <si>
+    <t>The test result for qualitative detection of (IgM / IgA) combined antibodies.</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1097,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1290,146 +1302,168 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="C26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="C27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="C30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>